<commit_message>
UX: select default values from well known values
</commit_message>
<xml_diff>
--- a/UnitTests/CarnassialData.Carnassial.UnitTests.DatabaseTests.RoundtripSpreadsheets.FilesToMerge.xlsx
+++ b/UnitTests/CarnassialData.Carnassial.UnitTests.DatabaseTests.RoundtripSpreadsheets.FilesToMerge.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todd\Documents\wildlife bio\Carnassial\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EA448264-B559-459F-9F55-25D9D69FF377}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2649F1D8-A29B-4A48-AEF2-D5B7BE4BC84E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>File</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Counter3Markers</t>
+  </si>
+  <si>
+    <t>choice b</t>
+  </si>
+  <si>
+    <t>Genus species</t>
   </si>
 </sst>
 </file>
@@ -971,7 +977,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,11 +1084,17 @@
       <c r="G2">
         <v>0</v>
       </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
       <c r="K2" t="b">
         <v>0</v>
       </c>
       <c r="L2">
         <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
       </c>
       <c r="P2" t="b">
         <v>1</v>
@@ -1125,6 +1137,9 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
       <c r="J3" t="s">
         <v>27</v>
       </c>
@@ -1133,6 +1148,9 @@
       </c>
       <c r="L3">
         <v>100</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
data: conform to SQLite best practice in handling column names
</commit_message>
<xml_diff>
--- a/UnitTests/CarnassialData.Carnassial.UnitTests.DatabaseTests.RoundtripSpreadsheets.FilesToMerge.xlsx
+++ b/UnitTests/CarnassialData.Carnassial.UnitTests.DatabaseTests.RoundtripSpreadsheets.FilesToMerge.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todd\Documents\wildlife bio\Carnassial\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2649F1D8-A29B-4A48-AEF2-D5B7BE4BC84E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE59B6-0537-4D1D-A58E-31B30DF636F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,18 +49,6 @@
     <t>Flag0</t>
   </si>
   <si>
-    <t>CounterWithCustomDataLabel</t>
-  </si>
-  <si>
-    <t>ChoiceWithCustomDataLabel</t>
-  </si>
-  <si>
-    <t>NoteWithCustomDataLabel</t>
-  </si>
-  <si>
-    <t>FlagWithCustomDataLabel</t>
-  </si>
-  <si>
     <t>CounterNotVisible</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t>Counter0Markers</t>
   </si>
   <si>
-    <t>CounterWithCustomDataLabelMarkers</t>
-  </si>
-  <si>
     <t>CounterNotVisibleMarkers</t>
   </si>
   <si>
@@ -134,6 +119,21 @@
   </si>
   <si>
     <t>Genus species</t>
+  </si>
+  <si>
+    <t>कस्टम डेटा लेबल के साथ काउंटर</t>
+  </si>
+  <si>
+    <t>कस्टम डेटा लेबल के साथ काउंटरMarkers</t>
+  </si>
+  <si>
+    <t>カスタムデータラベルのフラグ</t>
+  </si>
+  <si>
+    <t>注意使用自定义数据标签</t>
+  </si>
+  <si>
+    <t>Bandera con"etiqueta"de"datos personalizada</t>
   </si>
 </sst>
 </file>
@@ -977,7 +977,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1005,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -1017,66 +1017,66 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>16</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>-8</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -1094,7 +1094,7 @@
         <v>100</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P2" t="b">
         <v>1</v>
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Z2" t="b">
         <v>0</v>
@@ -1117,19 +1117,19 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
       </c>
       <c r="D3">
         <v>-8</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1138,10 +1138,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -1150,7 +1150,7 @@
         <v>100</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>
@@ -1159,7 +1159,7 @@
         <v>3</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="U3" t="b">
         <v>0</v>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Z3" t="b">
         <v>0</v>

</xml_diff>